<commit_message>
progress in revenue and costs
</commit_message>
<xml_diff>
--- a/output/emission_analysis.xlsx
+++ b/output/emission_analysis.xlsx
@@ -486,7 +486,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:ALL28"/>
+  <dimension ref="A2:ALL19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
@@ -500,14 +500,9 @@
     <col width="23" customWidth="1" min="3" max="3"/>
     <col width="2" customWidth="1" min="4" max="4"/>
     <col width="2" customWidth="1" min="6" max="6"/>
-    <col width="2" customWidth="1" min="9" max="9"/>
+    <col width="2" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="9" max="9"/>
     <col width="13" customWidth="1" min="10" max="10"/>
-    <col width="13" customWidth="1" min="11" max="11"/>
-    <col width="13" customWidth="1" min="12" max="12"/>
-    <col width="13" customWidth="1" min="13" max="13"/>
-    <col width="13" customWidth="1" min="14" max="14"/>
-    <col width="13" customWidth="1" min="15" max="15"/>
-    <col width="13" customWidth="1" min="16" max="16"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -2531,44 +2526,14 @@
           <t>2023-10</t>
         </is>
       </c>
-      <c r="H5" s="3" t="inlineStr">
-        <is>
-          <t>2023-11</t>
-        </is>
-      </c>
-      <c r="J5" s="3" t="inlineStr">
+      <c r="I5" s="3" t="inlineStr">
         <is>
           <t>2023 - wk 39</t>
         </is>
       </c>
-      <c r="K5" s="3" t="inlineStr">
+      <c r="J5" s="3" t="inlineStr">
         <is>
           <t>2023 - wk 40</t>
-        </is>
-      </c>
-      <c r="L5" s="3" t="inlineStr">
-        <is>
-          <t>2023 - wk 41</t>
-        </is>
-      </c>
-      <c r="M5" s="3" t="inlineStr">
-        <is>
-          <t>2023 - wk 42</t>
-        </is>
-      </c>
-      <c r="N5" s="3" t="inlineStr">
-        <is>
-          <t>2023 - wk 43</t>
-        </is>
-      </c>
-      <c r="O5" s="3" t="inlineStr">
-        <is>
-          <t>2023 - wk 44</t>
-        </is>
-      </c>
-      <c r="P5" s="3" t="inlineStr">
-        <is>
-          <t>2023 - wk 45</t>
         </is>
       </c>
     </row>
@@ -2582,34 +2547,16 @@
         </is>
       </c>
       <c r="E7" s="5" t="n">
-        <v>243341.5722382834</v>
+        <v>24881.33863753015</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>182964.3565130286</v>
-      </c>
-      <c r="H7" s="5" t="n">
-        <v>60377.21572525475</v>
+        <v>24881.33863753015</v>
+      </c>
+      <c r="I7" s="5" t="n">
+        <v>5941.27715589603</v>
       </c>
       <c r="J7" s="5" t="n">
-        <v>5788.839010501635</v>
-      </c>
-      <c r="K7" s="5" t="n">
-        <v>41045.00982550369</v>
-      </c>
-      <c r="L7" s="5" t="n">
-        <v>41235.60883514557</v>
-      </c>
-      <c r="M7" s="5" t="n">
-        <v>41122.08601394689</v>
-      </c>
-      <c r="N7" s="5" t="n">
-        <v>41229.61297387876</v>
-      </c>
-      <c r="O7" s="5" t="n">
-        <v>40731.88577359835</v>
-      </c>
-      <c r="P7" s="5" t="n">
-        <v>32188.52980570848</v>
+        <v>18940.06148163411</v>
       </c>
     </row>
     <row r="8">
@@ -2621,34 +2568,16 @@
         </is>
       </c>
       <c r="E8" s="7" t="n">
-        <v>205062.0426615557</v>
+        <v>22852.92280171143</v>
       </c>
       <c r="G8" s="7" t="n">
-        <v>154494.9669683367</v>
-      </c>
-      <c r="H8" s="7" t="n">
-        <v>50567.07569321899</v>
+        <v>22852.92280171143</v>
+      </c>
+      <c r="I8" s="7" t="n">
+        <v>5464.593570077317</v>
       </c>
       <c r="J8" s="7" t="n">
-        <v>4912.998432285264</v>
-      </c>
-      <c r="K8" s="7" t="n">
-        <v>34605.94551892477</v>
-      </c>
-      <c r="L8" s="7" t="n">
-        <v>34795.60190147579</v>
-      </c>
-      <c r="M8" s="7" t="n">
-        <v>34691.42805646258</v>
-      </c>
-      <c r="N8" s="7" t="n">
-        <v>34783.01924217368</v>
-      </c>
-      <c r="O8" s="7" t="n">
-        <v>34280.45329971881</v>
-      </c>
-      <c r="P8" s="7" t="n">
-        <v>26992.59621051481</v>
+        <v>17388.32923163411</v>
       </c>
     </row>
     <row r="9">
@@ -2665,28 +2594,10 @@
       <c r="G9" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="H9" s="7" t="n">
+      <c r="I9" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J9" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2695,37 +2606,19 @@
       <c r="B10" s="6" t="n"/>
       <c r="C10" s="6" t="inlineStr">
         <is>
-          <t>pv2_emissions</t>
+          <t>bat1_emissions</t>
         </is>
       </c>
       <c r="E10" s="7" t="n">
-        <v>0</v>
+        <v>0.05277777777777775</v>
       </c>
       <c r="G10" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="7" t="n">
-        <v>0</v>
+        <v>0.05277777777777775</v>
+      </c>
+      <c r="I10" s="7" t="n">
+        <v>0.05277777777777775</v>
       </c>
       <c r="J10" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N10" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P10" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2734,38 +2627,20 @@
       <c r="B11" s="6" t="n"/>
       <c r="C11" s="6" t="inlineStr">
         <is>
-          <t>bat1_emissions</t>
+          <t>CHP1_emissions</t>
         </is>
       </c>
       <c r="E11" s="7" t="n">
-        <v>0.05277777777777773</v>
+        <v>1485</v>
       </c>
       <c r="G11" s="7" t="n">
-        <v>0.05277777777777773</v>
-      </c>
-      <c r="H11" s="7" t="n">
-        <v>0</v>
+        <v>1485</v>
+      </c>
+      <c r="I11" s="7" t="n">
+        <v>345.0000000000001</v>
       </c>
       <c r="J11" s="7" t="n">
-        <v>0.05277777777777773</v>
-      </c>
-      <c r="K11" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L11" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N11" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O11" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P11" s="7" t="n">
-        <v>0</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="12">
@@ -2773,37 +2648,19 @@
       <c r="B12" s="6" t="n"/>
       <c r="C12" s="6" t="inlineStr">
         <is>
-          <t>bat2_emissions</t>
+          <t>solar_th1_emissions</t>
         </is>
       </c>
       <c r="E12" s="7" t="n">
-        <v>0.05277777777777773</v>
+        <v>0</v>
       </c>
       <c r="G12" s="7" t="n">
-        <v>0.05277777777777773</v>
-      </c>
-      <c r="H12" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="I12" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="J12" s="7" t="n">
-        <v>0.05277777777777773</v>
-      </c>
-      <c r="K12" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2812,38 +2669,20 @@
       <c r="B13" s="6" t="n"/>
       <c r="C13" s="6" t="inlineStr">
         <is>
-          <t>CHP1_emissions</t>
+          <t>pvt1_emissions</t>
         </is>
       </c>
       <c r="E13" s="7" t="n">
-        <v>14985</v>
+        <v>0</v>
       </c>
       <c r="G13" s="7" t="n">
-        <v>11145</v>
-      </c>
-      <c r="H13" s="7" t="n">
-        <v>3840</v>
+        <v>0</v>
+      </c>
+      <c r="I13" s="7" t="n">
+        <v>0</v>
       </c>
       <c r="J13" s="7" t="n">
-        <v>345</v>
-      </c>
-      <c r="K13" s="7" t="n">
-        <v>2520</v>
-      </c>
-      <c r="L13" s="7" t="n">
-        <v>2520</v>
-      </c>
-      <c r="M13" s="7" t="n">
-        <v>2520</v>
-      </c>
-      <c r="N13" s="7" t="n">
-        <v>2520</v>
-      </c>
-      <c r="O13" s="7" t="n">
-        <v>2520</v>
-      </c>
-      <c r="P13" s="7" t="n">
-        <v>2040</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -2851,38 +2690,20 @@
       <c r="B14" s="6" t="n"/>
       <c r="C14" s="6" t="inlineStr">
         <is>
-          <t>CHP2_emissions</t>
+          <t>charging_station1_emissions</t>
         </is>
       </c>
       <c r="E14" s="7" t="n">
-        <v>14985</v>
+        <v>126.468175</v>
       </c>
       <c r="G14" s="7" t="n">
-        <v>11145</v>
-      </c>
-      <c r="H14" s="7" t="n">
-        <v>3840</v>
+        <v>126.468175</v>
+      </c>
+      <c r="I14" s="7" t="n">
+        <v>34.73592500000001</v>
       </c>
       <c r="J14" s="7" t="n">
-        <v>345</v>
-      </c>
-      <c r="K14" s="7" t="n">
-        <v>2520</v>
-      </c>
-      <c r="L14" s="7" t="n">
-        <v>2520</v>
-      </c>
-      <c r="M14" s="7" t="n">
-        <v>2520</v>
-      </c>
-      <c r="N14" s="7" t="n">
-        <v>2520</v>
-      </c>
-      <c r="O14" s="7" t="n">
-        <v>2520</v>
-      </c>
-      <c r="P14" s="7" t="n">
-        <v>2040</v>
+        <v>91.73225000000002</v>
       </c>
     </row>
     <row r="15">
@@ -2890,7 +2711,7 @@
       <c r="B15" s="6" t="n"/>
       <c r="C15" s="6" t="inlineStr">
         <is>
-          <t>solar_th1_emissions</t>
+          <t>heat_pump1_emissions</t>
         </is>
       </c>
       <c r="E15" s="7" t="n">
@@ -2899,28 +2720,10 @@
       <c r="G15" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="H15" s="7" t="n">
+      <c r="I15" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J15" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L15" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M15" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P15" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2929,37 +2732,19 @@
       <c r="B16" s="6" t="n"/>
       <c r="C16" s="6" t="inlineStr">
         <is>
-          <t>solar_th2_emissions</t>
+          <t>bat_with_aging1_emissions</t>
         </is>
       </c>
       <c r="E16" s="7" t="n">
-        <v>0</v>
+        <v>0.05277777777777776</v>
       </c>
       <c r="G16" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" s="7" t="n">
-        <v>0</v>
+        <v>0.05277777777777776</v>
+      </c>
+      <c r="I16" s="7" t="n">
+        <v>0.05277777777777776</v>
       </c>
       <c r="J16" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K16" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L16" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M16" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N16" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O16" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P16" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2968,428 +2753,41 @@
       <c r="B17" s="6" t="n"/>
       <c r="C17" s="6" t="inlineStr">
         <is>
-          <t>pvt1_emissions</t>
+          <t>gas_boiler1_emissions</t>
         </is>
       </c>
       <c r="E17" s="7" t="n">
-        <v>0</v>
+        <v>416.842105263158</v>
       </c>
       <c r="G17" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="7" t="n">
-        <v>0</v>
+        <v>416.842105263158</v>
+      </c>
+      <c r="I17" s="7" t="n">
+        <v>96.8421052631579</v>
       </c>
       <c r="J17" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K17" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L17" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M17" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N17" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O17" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P17" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="6" t="n"/>
-      <c r="B18" s="6" t="n"/>
-      <c r="C18" s="6" t="inlineStr">
-        <is>
-          <t>pvt2_emissions</t>
-        </is>
-      </c>
-      <c r="E18" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J18" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K18" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L18" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M18" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O18" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P18" s="7" t="n">
-        <v>0</v>
+        <v>320.0000000000001</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="6" t="n"/>
-      <c r="B19" s="6" t="n"/>
-      <c r="C19" s="6" t="inlineStr">
-        <is>
-          <t>charging_station1_emissions</t>
-        </is>
-      </c>
-      <c r="E19" s="7" t="n">
-        <v>1304.808883333334</v>
-      </c>
-      <c r="G19" s="7" t="n">
-        <v>959.3789500000003</v>
-      </c>
-      <c r="H19" s="7" t="n">
-        <v>345.4299333333334</v>
-      </c>
-      <c r="J19" s="7" t="n">
-        <v>26.82118333333334</v>
-      </c>
-      <c r="K19" s="7" t="n">
-        <v>220.653225</v>
-      </c>
-      <c r="L19" s="7" t="n">
-        <v>219.9715083333334</v>
-      </c>
-      <c r="M19" s="7" t="n">
-        <v>211.96875</v>
-      </c>
-      <c r="N19" s="7" t="n">
-        <v>217.9037833333334</v>
-      </c>
-      <c r="O19" s="7" t="n">
-        <v>222.3256166666667</v>
-      </c>
-      <c r="P19" s="7" t="n">
-        <v>185.1648166666667</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="6" t="n"/>
-      <c r="B20" s="6" t="n"/>
-      <c r="C20" s="6" t="inlineStr">
-        <is>
-          <t>charging_station2_emissions</t>
-        </is>
-      </c>
-      <c r="E20" s="7" t="n">
-        <v>817.6082083333336</v>
-      </c>
-      <c r="G20" s="7" t="n">
-        <v>616.5107250000002</v>
-      </c>
-      <c r="H20" s="7" t="n">
-        <v>201.0974833333334</v>
-      </c>
-      <c r="J20" s="7" t="n">
-        <v>24.07144166666668</v>
-      </c>
-      <c r="K20" s="7" t="n">
-        <v>133.35845</v>
-      </c>
-      <c r="L20" s="7" t="n">
-        <v>134.6838</v>
-      </c>
-      <c r="M20" s="7" t="n">
-        <v>133.1940666666667</v>
-      </c>
-      <c r="N20" s="7" t="n">
-        <v>143.275925</v>
-      </c>
-      <c r="O20" s="7" t="n">
-        <v>143.9736250000001</v>
-      </c>
-      <c r="P20" s="7" t="n">
-        <v>105.0509</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="6" t="n"/>
-      <c r="B21" s="6" t="n"/>
-      <c r="C21" s="6" t="inlineStr">
-        <is>
-          <t>heat_pump1_emissions</t>
-        </is>
-      </c>
-      <c r="E21" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G21" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H21" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L21" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M21" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N21" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O21" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P21" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="6" t="n"/>
-      <c r="B22" s="6" t="n"/>
-      <c r="C22" s="6" t="inlineStr">
-        <is>
-          <t>heat_pump2_emissions</t>
-        </is>
-      </c>
-      <c r="E22" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K22" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L22" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M22" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N22" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O22" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P22" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="6" t="n"/>
-      <c r="B23" s="6" t="n"/>
-      <c r="C23" s="6" t="inlineStr">
-        <is>
-          <t>bat_with_aging1_emissions</t>
-        </is>
-      </c>
-      <c r="E23" s="7" t="n">
-        <v>0.05277777777777776</v>
-      </c>
-      <c r="G23" s="7" t="n">
-        <v>0.05277777777777776</v>
-      </c>
-      <c r="H23" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J23" s="7" t="n">
-        <v>0.05277777777777776</v>
-      </c>
-      <c r="K23" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L23" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M23" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N23" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O23" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P23" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="6" t="n"/>
-      <c r="B24" s="6" t="n"/>
-      <c r="C24" s="6" t="inlineStr">
-        <is>
-          <t>bat_with_aging2_emissions</t>
-        </is>
-      </c>
-      <c r="E24" s="7" t="n">
-        <v>0.05277777777777776</v>
-      </c>
-      <c r="G24" s="7" t="n">
-        <v>0.05277777777777776</v>
-      </c>
-      <c r="H24" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J24" s="7" t="n">
-        <v>0.05277777777777776</v>
-      </c>
-      <c r="K24" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L24" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M24" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N24" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O24" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P24" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="6" t="n"/>
-      <c r="B25" s="6" t="n"/>
-      <c r="C25" s="6" t="inlineStr">
-        <is>
-          <t>gas_boiler1_emissions</t>
-        </is>
-      </c>
-      <c r="E25" s="7" t="n">
-        <v>3094.189194368667</v>
-      </c>
-      <c r="G25" s="7" t="n">
-        <v>2302.155526367974</v>
-      </c>
-      <c r="H25" s="7" t="n">
-        <v>792.0336680006928</v>
-      </c>
-      <c r="J25" s="7" t="n">
-        <v>67.3684210526289</v>
-      </c>
-      <c r="K25" s="7" t="n">
-        <v>522.5263157894589</v>
-      </c>
-      <c r="L25" s="7" t="n">
-        <v>522.8253095469844</v>
-      </c>
-      <c r="M25" s="7" t="n">
-        <v>522.9688250281929</v>
-      </c>
-      <c r="N25" s="7" t="n">
-        <v>522.8877075822928</v>
-      </c>
-      <c r="O25" s="7" t="n">
-        <v>522.5263157894589</v>
-      </c>
-      <c r="P25" s="7" t="n">
-        <v>413.0862995796505</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="6" t="n"/>
-      <c r="B26" s="6" t="n"/>
-      <c r="C26" s="6" t="inlineStr">
-        <is>
-          <t>gas_boiler2_emissions</t>
-        </is>
-      </c>
-      <c r="E26" s="7" t="n">
-        <v>3092.712179581232</v>
-      </c>
-      <c r="G26" s="7" t="n">
-        <v>2301.13323221283</v>
-      </c>
-      <c r="H26" s="7" t="n">
-        <v>791.5789473684016</v>
-      </c>
-      <c r="J26" s="7" t="n">
-        <v>67.36842105262967</v>
-      </c>
-      <c r="K26" s="7" t="n">
-        <v>522.5263157894589</v>
-      </c>
-      <c r="L26" s="7" t="n">
-        <v>522.5263157894589</v>
-      </c>
-      <c r="M26" s="7" t="n">
-        <v>522.5263157894592</v>
-      </c>
-      <c r="N26" s="7" t="n">
-        <v>522.5263157894592</v>
-      </c>
-      <c r="O26" s="7" t="n">
-        <v>522.6069164234074</v>
-      </c>
-      <c r="P26" s="7" t="n">
-        <v>412.6315789473585</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="4" t="n"/>
-      <c r="B28" s="4" t="n"/>
-      <c r="C28" s="4" t="inlineStr">
+      <c r="A19" s="4" t="n"/>
+      <c r="B19" s="4" t="n"/>
+      <c r="C19" s="4" t="inlineStr">
         <is>
           <t>2 - Emissions accumulated</t>
         </is>
       </c>
-      <c r="E28" s="5" t="n">
-        <v>243341.5722382834</v>
-      </c>
-      <c r="G28" s="5" t="n">
-        <v>182964.3565130286</v>
-      </c>
-      <c r="H28" s="5" t="n">
-        <v>243341.5722382834</v>
-      </c>
-      <c r="J28" s="5" t="n">
-        <v>5788.839010501635</v>
-      </c>
-      <c r="K28" s="5" t="n">
-        <v>46833.84883600533</v>
-      </c>
-      <c r="L28" s="5" t="n">
-        <v>88069.4576711509</v>
-      </c>
-      <c r="M28" s="5" t="n">
-        <v>129191.5436850978</v>
-      </c>
-      <c r="N28" s="5" t="n">
-        <v>170421.1566589766</v>
-      </c>
-      <c r="O28" s="5" t="n">
-        <v>211153.0424325749</v>
-      </c>
-      <c r="P28" s="5" t="n">
-        <v>243341.5722382834</v>
+      <c r="E19" s="5" t="n">
+        <v>24881.33863753015</v>
+      </c>
+      <c r="G19" s="5" t="n">
+        <v>24881.33863753015</v>
+      </c>
+      <c r="I19" s="5" t="n">
+        <v>5941.27715589603</v>
+      </c>
+      <c r="J19" s="5" t="n">
+        <v>24881.33863753014</v>
       </c>
     </row>
   </sheetData>

</xml_diff>